<commit_message>
Add API Login/ Register.
</commit_message>
<xml_diff>
--- a/APIs.xlsx
+++ b/APIs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12330"/>
+    <workbookView windowWidth="21240" windowHeight="8760"/>
   </bookViews>
   <sheets>
     <sheet name="API_List" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>Planing API</t>
   </si>
@@ -71,7 +71,10 @@
     <t>Add more tables, entities, define strategy for authorization</t>
   </si>
   <si>
-    <t>Add common security, filter chain, messageSource config, jdbc template config, exception handler</t>
+    <t>Multiple message, Controller Advice (message validation), datasource config</t>
+  </si>
+  <si>
+    <t>Add common security</t>
   </si>
   <si>
     <t>Start API for admin</t>
@@ -88,7 +91,7 @@
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,13 +111,6 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -650,148 +646,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1156,8 +1152,8 @@
   <sheetPr/>
   <dimension ref="B2:T76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53:S53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1626,9 +1622,7 @@
         <v>45267</v>
       </c>
       <c r="D51" s="12"/>
-      <c r="E51" s="13" t="s">
-        <v>18</v>
-      </c>
+      <c r="E51" s="13"/>
       <c r="F51" s="13"/>
       <c r="G51" s="13"/>
       <c r="H51" s="13"/>
@@ -1651,9 +1645,7 @@
         <v>45268</v>
       </c>
       <c r="D52" s="12"/>
-      <c r="E52" s="13" t="s">
-        <v>18</v>
-      </c>
+      <c r="E52" s="13"/>
       <c r="F52" s="13"/>
       <c r="G52" s="13"/>
       <c r="H52" s="13"/>
@@ -1702,7 +1694,7 @@
       </c>
       <c r="D54" s="12"/>
       <c r="E54" s="13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F54" s="13"/>
       <c r="G54" s="13"/>
@@ -1727,7 +1719,7 @@
       </c>
       <c r="D55" s="12"/>
       <c r="E55" s="13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F55" s="13"/>
       <c r="G55" s="13"/>
@@ -1752,7 +1744,7 @@
       </c>
       <c r="D56" s="12"/>
       <c r="E56" s="13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F56" s="13"/>
       <c r="G56" s="13"/>

</xml_diff>

<commit_message>
ADD API For admin
</commit_message>
<xml_diff>
--- a/APIs.xlsx
+++ b/APIs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21240" windowHeight="8760"/>
+    <workbookView windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="API_List" sheetId="1" r:id="rId1"/>
@@ -14,18 +14,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>Planing API</t>
   </si>
   <si>
+    <t>Common DB</t>
+  </si>
+  <si>
     <t>Admin</t>
   </si>
   <si>
+    <t>Name</t>
+  </si>
+  <si>
     <t>Product</t>
   </si>
   <si>
+    <t>Title</t>
+  </si>
+  <si>
     <t>CRUD</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>TEXT</t>
+  </si>
+  <si>
+    <t>DeleteFG</t>
+  </si>
+  <si>
+    <t>Default false</t>
+  </si>
+  <si>
+    <t>Not null</t>
   </si>
   <si>
     <t>Category</t>
@@ -77,7 +101,10 @@
     <t>Add common security</t>
   </si>
   <si>
-    <t>Start API for admin</t>
+    <t>Start API for admin (category, product)</t>
+  </si>
+  <si>
+    <t>Search Product with multi conditions</t>
   </si>
 </sst>
 </file>
@@ -1150,10 +1177,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B2:T76"/>
+  <dimension ref="B2:AO76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53:S53"/>
+    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
+      <selection activeCell="E60" sqref="E60:S60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1164,7 +1191,7 @@
   </cols>
   <sheetData>
     <row r="2" ht="15.75"/>
-    <row r="3" spans="2:20">
+    <row r="3" spans="2:41">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1186,8 +1213,29 @@
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
       <c r="T3" s="14"/>
-    </row>
-    <row r="4" spans="2:20">
+      <c r="W3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AE3" s="3"/>
+      <c r="AF3" s="3"/>
+      <c r="AG3" s="3"/>
+      <c r="AH3" s="3"/>
+      <c r="AI3" s="3"/>
+      <c r="AJ3" s="3"/>
+      <c r="AK3" s="3"/>
+      <c r="AL3" s="3"/>
+      <c r="AM3" s="3"/>
+      <c r="AN3" s="3"/>
+      <c r="AO3" s="14"/>
+    </row>
+    <row r="4" spans="2:41">
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -1207,8 +1255,27 @@
       <c r="R4" s="5"/>
       <c r="S4" s="5"/>
       <c r="T4" s="15"/>
-    </row>
-    <row r="5" spans="2:20">
+      <c r="W4" s="4"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="5"/>
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="5"/>
+      <c r="AC4" s="5"/>
+      <c r="AD4" s="5"/>
+      <c r="AE4" s="5"/>
+      <c r="AF4" s="5"/>
+      <c r="AG4" s="5"/>
+      <c r="AH4" s="5"/>
+      <c r="AI4" s="5"/>
+      <c r="AJ4" s="5"/>
+      <c r="AK4" s="5"/>
+      <c r="AL4" s="5"/>
+      <c r="AM4" s="5"/>
+      <c r="AN4" s="5"/>
+      <c r="AO4" s="15"/>
+    </row>
+    <row r="5" spans="2:41">
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -1228,8 +1295,27 @@
       <c r="R5" s="5"/>
       <c r="S5" s="5"/>
       <c r="T5" s="15"/>
-    </row>
-    <row r="6" ht="15.75" spans="2:20">
+      <c r="W5" s="4"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="5"/>
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="5"/>
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="5"/>
+      <c r="AE5" s="5"/>
+      <c r="AF5" s="5"/>
+      <c r="AG5" s="5"/>
+      <c r="AH5" s="5"/>
+      <c r="AI5" s="5"/>
+      <c r="AJ5" s="5"/>
+      <c r="AK5" s="5"/>
+      <c r="AL5" s="5"/>
+      <c r="AM5" s="5"/>
+      <c r="AN5" s="5"/>
+      <c r="AO5" s="15"/>
+    </row>
+    <row r="6" ht="15.75" spans="2:41">
       <c r="B6" s="6"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -1249,187 +1335,300 @@
       <c r="R6" s="7"/>
       <c r="S6" s="7"/>
       <c r="T6" s="16"/>
-    </row>
-    <row r="7" spans="2:20">
+      <c r="W6" s="6"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="7"/>
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="7"/>
+      <c r="AC6" s="7"/>
+      <c r="AD6" s="7"/>
+      <c r="AE6" s="7"/>
+      <c r="AF6" s="7"/>
+      <c r="AG6" s="7"/>
+      <c r="AH6" s="7"/>
+      <c r="AI6" s="7"/>
+      <c r="AJ6" s="7"/>
+      <c r="AK6" s="7"/>
+      <c r="AL6" s="7"/>
+      <c r="AM6" s="7"/>
+      <c r="AN6" s="7"/>
+      <c r="AO6" s="16"/>
+    </row>
+    <row r="7" spans="2:41">
       <c r="B7" s="8"/>
       <c r="T7" s="17"/>
-    </row>
-    <row r="8" spans="2:20">
+      <c r="W7" s="8"/>
+      <c r="AO7" s="17"/>
+    </row>
+    <row r="8" spans="2:41">
       <c r="B8" s="8"/>
       <c r="C8" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T8" s="17"/>
-    </row>
-    <row r="9" spans="2:20">
+      <c r="W8" s="8"/>
+      <c r="X8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z8" s="1">
+        <v>50</v>
+      </c>
+      <c r="AB8" s="1">
+        <v>255</v>
+      </c>
+      <c r="AO8" s="17"/>
+    </row>
+    <row r="9" spans="2:41">
       <c r="B9" s="8"/>
       <c r="D9" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T9" s="17"/>
-    </row>
-    <row r="10" spans="2:20">
+      <c r="W9" s="8"/>
+      <c r="X9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z9" s="1">
+        <v>255</v>
+      </c>
+      <c r="AB9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AO9" s="17"/>
+    </row>
+    <row r="10" spans="2:41">
       <c r="B10" s="8"/>
       <c r="E10" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="T10" s="17"/>
-    </row>
-    <row r="11" spans="2:20">
+      <c r="W10" s="8"/>
+      <c r="X10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z10" s="1">
+        <v>10000</v>
+      </c>
+      <c r="AB10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AO10" s="17"/>
+    </row>
+    <row r="11" spans="2:41">
       <c r="B11" s="8"/>
       <c r="T11" s="17"/>
-    </row>
-    <row r="12" spans="2:20">
+      <c r="W11" s="8"/>
+      <c r="X11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AO11" s="17"/>
+    </row>
+    <row r="12" spans="2:41">
       <c r="B12" s="8"/>
       <c r="D12" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="T12" s="17"/>
-    </row>
-    <row r="13" spans="2:20">
+      <c r="W12" s="8"/>
+      <c r="AO12" s="17"/>
+    </row>
+    <row r="13" spans="2:41">
       <c r="B13" s="8"/>
       <c r="E13" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="T13" s="17"/>
-    </row>
-    <row r="14" spans="2:20">
+      <c r="W13" s="8"/>
+      <c r="AO13" s="17"/>
+    </row>
+    <row r="14" spans="2:41">
       <c r="B14" s="8"/>
       <c r="T14" s="17"/>
-    </row>
-    <row r="15" spans="2:20">
+      <c r="W14" s="8"/>
+      <c r="AO14" s="17"/>
+    </row>
+    <row r="15" spans="2:41">
       <c r="B15" s="8"/>
       <c r="D15" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="T15" s="17"/>
-    </row>
-    <row r="16" spans="2:20">
+      <c r="W15" s="8"/>
+      <c r="AO15" s="17"/>
+    </row>
+    <row r="16" spans="2:41">
       <c r="B16" s="8"/>
       <c r="E16" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="T16" s="17"/>
-    </row>
-    <row r="17" spans="2:20">
+      <c r="W16" s="8"/>
+      <c r="AO16" s="17"/>
+    </row>
+    <row r="17" spans="2:41">
       <c r="B17" s="8"/>
       <c r="T17" s="17"/>
-    </row>
-    <row r="18" spans="2:20">
+      <c r="W17" s="8"/>
+      <c r="AO17" s="17"/>
+    </row>
+    <row r="18" spans="2:41">
       <c r="B18" s="8"/>
       <c r="T18" s="17"/>
-    </row>
-    <row r="19" spans="2:20">
+      <c r="W18" s="8"/>
+      <c r="AO18" s="17"/>
+    </row>
+    <row r="19" spans="2:41">
       <c r="B19" s="8"/>
       <c r="C19" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="T19" s="17"/>
-    </row>
-    <row r="20" spans="2:20">
+      <c r="W19" s="8"/>
+      <c r="AO19" s="17"/>
+    </row>
+    <row r="20" spans="2:41">
       <c r="B20" s="8"/>
       <c r="D20" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T20" s="17"/>
-    </row>
-    <row r="21" spans="2:20">
+      <c r="W20" s="8"/>
+      <c r="AO20" s="17"/>
+    </row>
+    <row r="21" spans="2:41">
       <c r="B21" s="8"/>
       <c r="E21" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="T21" s="17"/>
-    </row>
-    <row r="22" spans="2:20">
+      <c r="W21" s="8"/>
+      <c r="AO21" s="17"/>
+    </row>
+    <row r="22" spans="2:41">
       <c r="B22" s="8"/>
       <c r="T22" s="17"/>
-    </row>
-    <row r="23" spans="2:20">
+      <c r="W22" s="8"/>
+      <c r="AO22" s="17"/>
+    </row>
+    <row r="23" spans="2:41">
       <c r="B23" s="8"/>
       <c r="D23" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="T23" s="17"/>
-    </row>
-    <row r="24" spans="2:20">
+      <c r="W23" s="8"/>
+      <c r="AO23" s="17"/>
+    </row>
+    <row r="24" spans="2:41">
       <c r="B24" s="8"/>
       <c r="E24" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="T24" s="17"/>
-    </row>
-    <row r="25" spans="2:20">
+      <c r="W24" s="8"/>
+      <c r="AO24" s="17"/>
+    </row>
+    <row r="25" spans="2:41">
       <c r="B25" s="8"/>
       <c r="T25" s="17"/>
-    </row>
-    <row r="26" spans="2:20">
+      <c r="W25" s="8"/>
+      <c r="AO25" s="17"/>
+    </row>
+    <row r="26" spans="2:41">
       <c r="B26" s="8"/>
       <c r="D26" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="T26" s="17"/>
-    </row>
-    <row r="27" spans="2:20">
+      <c r="W26" s="8"/>
+      <c r="AO26" s="17"/>
+    </row>
+    <row r="27" spans="2:41">
       <c r="B27" s="8"/>
       <c r="E27" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="T27" s="17"/>
-    </row>
-    <row r="28" spans="2:20">
+      <c r="W27" s="8"/>
+      <c r="AO27" s="17"/>
+    </row>
+    <row r="28" spans="2:41">
       <c r="B28" s="8"/>
       <c r="E28" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="T28" s="17"/>
-    </row>
-    <row r="29" spans="2:20">
+      <c r="W28" s="8"/>
+      <c r="AO28" s="17"/>
+    </row>
+    <row r="29" spans="2:41">
       <c r="B29" s="8"/>
       <c r="D29" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="T29" s="17"/>
-    </row>
-    <row r="30" spans="2:20">
+      <c r="W29" s="8"/>
+      <c r="AO29" s="17"/>
+    </row>
+    <row r="30" spans="2:41">
       <c r="B30" s="8"/>
       <c r="E30" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="T30" s="17"/>
-    </row>
-    <row r="31" spans="2:20">
+      <c r="W30" s="8"/>
+      <c r="AO30" s="17"/>
+    </row>
+    <row r="31" spans="2:41">
       <c r="B31" s="8"/>
       <c r="D31" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="T31" s="17"/>
-    </row>
-    <row r="32" spans="2:20">
+      <c r="W31" s="8"/>
+      <c r="AO31" s="17"/>
+    </row>
+    <row r="32" spans="2:41">
       <c r="B32" s="8"/>
       <c r="E32" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="T32" s="17"/>
-    </row>
-    <row r="33" spans="2:20">
+      <c r="W32" s="8"/>
+      <c r="AO32" s="17"/>
+    </row>
+    <row r="33" spans="2:41">
       <c r="B33" s="8"/>
       <c r="D33" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="T33" s="17"/>
-    </row>
-    <row r="34" spans="2:20">
+      <c r="W33" s="8"/>
+      <c r="AO33" s="17"/>
+    </row>
+    <row r="34" spans="2:41">
       <c r="B34" s="8"/>
       <c r="E34" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="T34" s="17"/>
-    </row>
-    <row r="35" spans="2:20">
+      <c r="W34" s="8"/>
+      <c r="AO34" s="17"/>
+    </row>
+    <row r="35" spans="2:41">
       <c r="B35" s="8"/>
       <c r="T35" s="17"/>
-    </row>
-    <row r="36" ht="15.75" spans="2:20">
+      <c r="W35" s="8"/>
+      <c r="AO35" s="17"/>
+    </row>
+    <row r="36" ht="15.75" spans="2:41">
       <c r="B36" s="9"/>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
@@ -1449,11 +1648,30 @@
       <c r="R36" s="10"/>
       <c r="S36" s="10"/>
       <c r="T36" s="18"/>
+      <c r="W36" s="9"/>
+      <c r="X36" s="10"/>
+      <c r="Y36" s="10"/>
+      <c r="Z36" s="10"/>
+      <c r="AA36" s="10"/>
+      <c r="AB36" s="10"/>
+      <c r="AC36" s="10"/>
+      <c r="AD36" s="10"/>
+      <c r="AE36" s="10"/>
+      <c r="AF36" s="10"/>
+      <c r="AG36" s="10"/>
+      <c r="AH36" s="10"/>
+      <c r="AI36" s="10"/>
+      <c r="AJ36" s="10"/>
+      <c r="AK36" s="10"/>
+      <c r="AL36" s="10"/>
+      <c r="AM36" s="10"/>
+      <c r="AN36" s="10"/>
+      <c r="AO36" s="18"/>
     </row>
     <row r="42" ht="15.75"/>
     <row r="43" spans="2:20">
       <c r="B43" s="2" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
@@ -1548,7 +1766,7 @@
       </c>
       <c r="D48" s="12"/>
       <c r="E48" s="13" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="F48" s="13"/>
       <c r="G48" s="13"/>
@@ -1573,7 +1791,7 @@
       </c>
       <c r="D49" s="12"/>
       <c r="E49" s="13" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F49" s="13"/>
       <c r="G49" s="13"/>
@@ -1598,7 +1816,7 @@
       </c>
       <c r="D50" s="12"/>
       <c r="E50" s="13" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="F50" s="13"/>
       <c r="G50" s="13"/>
@@ -1669,7 +1887,7 @@
       </c>
       <c r="D53" s="12"/>
       <c r="E53" s="13" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F53" s="13"/>
       <c r="G53" s="13"/>
@@ -1694,7 +1912,7 @@
       </c>
       <c r="D54" s="12"/>
       <c r="E54" s="13" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F54" s="13"/>
       <c r="G54" s="13"/>
@@ -1719,7 +1937,7 @@
       </c>
       <c r="D55" s="12"/>
       <c r="E55" s="13" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F55" s="13"/>
       <c r="G55" s="13"/>
@@ -1743,23 +1961,6 @@
         <v>45272</v>
       </c>
       <c r="D56" s="12"/>
-      <c r="E56" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F56" s="13"/>
-      <c r="G56" s="13"/>
-      <c r="H56" s="13"/>
-      <c r="I56" s="13"/>
-      <c r="J56" s="13"/>
-      <c r="K56" s="13"/>
-      <c r="L56" s="13"/>
-      <c r="M56" s="13"/>
-      <c r="N56" s="13"/>
-      <c r="O56" s="13"/>
-      <c r="P56" s="13"/>
-      <c r="Q56" s="13"/>
-      <c r="R56" s="13"/>
-      <c r="S56" s="13"/>
       <c r="T56" s="17"/>
     </row>
     <row r="57" spans="2:20">
@@ -1768,21 +1969,6 @@
         <v>45273</v>
       </c>
       <c r="D57" s="12"/>
-      <c r="E57" s="13"/>
-      <c r="F57" s="13"/>
-      <c r="G57" s="13"/>
-      <c r="H57" s="13"/>
-      <c r="I57" s="13"/>
-      <c r="J57" s="13"/>
-      <c r="K57" s="13"/>
-      <c r="L57" s="13"/>
-      <c r="M57" s="13"/>
-      <c r="N57" s="13"/>
-      <c r="O57" s="13"/>
-      <c r="P57" s="13"/>
-      <c r="Q57" s="13"/>
-      <c r="R57" s="13"/>
-      <c r="S57" s="13"/>
       <c r="T57" s="17"/>
     </row>
     <row r="58" spans="2:20">
@@ -1814,7 +2000,9 @@
         <v>45275</v>
       </c>
       <c r="D59" s="12"/>
-      <c r="E59" s="13"/>
+      <c r="E59" s="13" t="s">
+        <v>28</v>
+      </c>
       <c r="F59" s="13"/>
       <c r="G59" s="13"/>
       <c r="H59" s="13"/>
@@ -1833,14 +2021,40 @@
     </row>
     <row r="60" spans="2:20">
       <c r="B60" s="8"/>
+      <c r="C60" s="11">
+        <v>45276</v>
+      </c>
+      <c r="E60" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F60" s="13"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="13"/>
+      <c r="I60" s="13"/>
+      <c r="J60" s="13"/>
+      <c r="K60" s="13"/>
+      <c r="L60" s="13"/>
+      <c r="M60" s="13"/>
+      <c r="N60" s="13"/>
+      <c r="O60" s="13"/>
+      <c r="P60" s="13"/>
+      <c r="Q60" s="13"/>
+      <c r="R60" s="13"/>
+      <c r="S60" s="13"/>
       <c r="T60" s="17"/>
     </row>
     <row r="61" spans="2:20">
       <c r="B61" s="8"/>
+      <c r="C61" s="11">
+        <v>45277</v>
+      </c>
       <c r="T61" s="17"/>
     </row>
     <row r="62" spans="2:20">
       <c r="B62" s="8"/>
+      <c r="C62" s="11">
+        <v>45278</v>
+      </c>
       <c r="T62" s="17"/>
     </row>
     <row r="63" spans="2:20">
@@ -1926,12 +2140,12 @@
     <mergeCell ref="E53:S53"/>
     <mergeCell ref="E54:S54"/>
     <mergeCell ref="E55:S55"/>
-    <mergeCell ref="E56:S56"/>
-    <mergeCell ref="E57:S57"/>
     <mergeCell ref="E58:S58"/>
     <mergeCell ref="E59:S59"/>
+    <mergeCell ref="E60:S60"/>
     <mergeCell ref="B3:T6"/>
     <mergeCell ref="B43:T46"/>
+    <mergeCell ref="W3:AO6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>